<commit_message>
changed theme of spreadsheet
</commit_message>
<xml_diff>
--- a/Astronomyhw.xlsx
+++ b/Astronomyhw.xlsx
@@ -263,9 +263,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Celestial">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Celestial">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -273,48 +273,48 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="18276C"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EBEBEB"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="AC3EC1"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="477BD1"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="46B298"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="90BA4C"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="DD9D31"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="E25247"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="C573D2"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="CCAEE8"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Celestial">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Angsana New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -343,13 +343,13 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Cordia New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -375,7 +375,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Celestial">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -384,23 +384,14 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="70000"/>
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="82000"/>
+                <a:alpha val="74000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -410,50 +401,38 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
+                <a:tint val="98000"/>
                 <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="88000"/>
+                <a:lumMod val="88000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="rnd" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="25400" cap="rnd" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -461,55 +440,64 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="63500" dist="38100" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="65000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="tl">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="38100" h="12700"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="90000"/>
+                <a:shade val="96000"/>
+                <a:hueMod val="100000"/>
+                <a:satMod val="180000"/>
+                <a:lumMod val="110000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="96000"/>
+                <a:satMod val="160000"/>
+                <a:lumMod val="100000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="4740000" scaled="1"/>
         </a:gradFill>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch/>
+        </a:blipFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
@@ -517,7 +505,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Celestial" id="{C4BB2A3D-0E93-4C5F-B0D2-9D3FCE089CC5}" vid="{42E5908D-19A2-46FD-89FA-638B126129EF}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -529,19 +517,19 @@
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="107" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H5" sqref="H5"/>
+      <selection pane="topRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.1640625" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
@@ -1004,5 +992,6 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>